<commit_message>
Update to the readme with new data
</commit_message>
<xml_diff>
--- a/resources/real_data.xlsx
+++ b/resources/real_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c6753fe18d1ac6c8/Documents/GitHub/tumor_ide_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c6753fe18d1ac6c8/Documents/GitHub/tumor_ide_project/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{84ACA977-A383-420E-B917-EFC70D735D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29F022DA-D0AD-494F-AD8E-051DFBA1D0FD}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{84ACA977-A383-420E-B917-EFC70D735D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{716F0029-0A04-4E85-9A4D-4A8A198461E2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,23 +77,23 @@
     <t>GO28753</t>
   </si>
   <si>
-    <t>NSCLC</t>
-  </si>
-  <si>
     <t>"Participants received docetaxel 75 milligram per meter square (mg/m^2) administered intravenously on Day 1 of each 21 day cycle until disease progression or unacceptable toxicity or death."</t>
   </si>
   <si>
-    <t>Non-Squamous NSCLC</t>
+    <t>"Docetaxel 75 milligrams per meter square (mg/m^2) was administered via IV infusion on Day 1 of each 21-day cycle until disease progression, death, unacceptable toxicity, withdrawal of consent, or study termination by sponsor, whichever occurs first."</t>
   </si>
   <si>
-    <t>"Docetaxel 75 milligrams per meter square (mg/m^2) was administered via IV infusion on Day 1 of each 21-day cycle until disease progression, death, unacceptable toxicity, withdrawal of consent, or study termination by sponsor, whichever occurs first."</t>
+    <t>"Advanced or metastatic non-small cell lung cancer after platinum failure"</t>
+  </si>
+  <si>
+    <t>"Locally advanced or metastatic non-small cell lung cancer (NSCLC) after failure with platinum-containing chemotherapy"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +114,14 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -154,10 +162,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -167,8 +176,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -310,10 +321,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A750873F-29DF-C742-8C0A-0FDAF55AF2CE}">
   <dimension ref="A1:G2853"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C380" workbookViewId="0">
+      <selection activeCell="G388" sqref="G388"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -630,7 +637,7 @@
     <col min="3" max="3" width="27.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -663,7 +670,7 @@
       <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -684,7 +691,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="58" x14ac:dyDescent="0.35">
@@ -701,7 +708,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -6054,14 +6061,14 @@
       <c r="E386" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F386" s="3" t="s">
+      <c r="F386" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G386" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="387" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A387">
         <v>8.1249219090499661E+17</v>
       </c>
@@ -6074,8 +6081,8 @@
       <c r="D387" t="s">
         <v>8</v>
       </c>
-      <c r="F387" t="s">
-        <v>16</v>
+      <c r="F387" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="388" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
@@ -6092,7 +6099,7 @@
         <v>8</v>
       </c>
       <c r="F388" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.35">
@@ -40602,9 +40609,13 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" location="study-plan" xr:uid="{8E642693-8FE0-461A-B9DA-C0BAA77671AB}"/>
+    <hyperlink ref="F386" r:id="rId2" location="study-plan" xr:uid="{B18CFF07-3152-475C-A1F2-519BCCDD974B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>